<commit_message>
Invoice dates + defaults
</commit_message>
<xml_diff>
--- a/ezeeparent/ezee_invoice_tracking.xlsx
+++ b/ezeeparent/ezee_invoice_tracking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Outstanding Tasks</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t>Add ability to encrypt/decrypt user sensitive data (acc name/number/bsb)</t>
+  </si>
+  <si>
+    <t>Disable delete/save buttons when doing DB operations</t>
+  </si>
+  <si>
+    <t>Add wait cursor on all delete/save operations</t>
+  </si>
+  <si>
+    <t>Add default 'manual tax' to DB configuration row</t>
+  </si>
+  <si>
+    <t>Add default 'debt age' to DB configuration row</t>
+  </si>
+  <si>
+    <t>Add default 'supplier' to invoice screen (add this default to the DB configuration row)</t>
+  </si>
+  <si>
+    <t>Setup confluence on ezeeit.com server and add basic instructions for ezee invoices</t>
+  </si>
+  <si>
+    <t>Add 'invoice date' to invoice entity (= date on the supplier invoice)</t>
+  </si>
+  <si>
+    <t>Add invoice date from/to search filter fields on the invoice grid</t>
+  </si>
+  <si>
+    <t>Ass invoice date to the grid model</t>
   </si>
 </sst>
 </file>
@@ -159,8 +186,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -177,18 +208,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -206,66 +241,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -636,7 +611,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -800,7 +775,7 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16" thickBot="1">
@@ -811,7 +786,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" thickBot="1">
@@ -822,7 +797,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" thickBot="1">
@@ -836,17 +811,116 @@
         <v>4</v>
       </c>
     </row>
+    <row r="19" spans="1:3" ht="16" thickBot="1">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" thickBot="1">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" thickBot="1">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" thickBot="1">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" thickBot="1">
+      <c r="A23" s="2">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" thickBot="1">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" thickBot="1">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16" thickBot="1">
+      <c r="A26" s="2">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16" thickBot="1">
+      <c r="A27" s="2">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C4:C19">
-    <cfRule type="expression" dxfId="11" priority="9">
+  <conditionalFormatting sqref="C4:C27">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>"Not Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C18">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+  <conditionalFormatting sqref="C4:C27">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>$T$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>$T$1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>